<commit_message>
More comprehensive tests for the lexer (comments, literals, expressions). Precedence file now has table to show which features are implemented by the parser and lexer, what the expected input and output of operators are, etc. Added lexer tes expected output. This will be checked against the test after any changes to ensure accuracy. Token toString() now print the type and is formatted. Parser now parsed functions. Lexer is reorganized.
</commit_message>
<xml_diff>
--- a/Precedence Rules.xlsx
+++ b/Precedence Rules.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Feature Tracking" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="125">
   <si>
     <t>Operators</t>
   </si>
@@ -99,9 +99,6 @@
     <t>negation</t>
   </si>
   <si>
-    <t>|x| () {} int()</t>
-  </si>
-  <si>
     <t>absolute value/grouping/casting</t>
   </si>
   <si>
@@ -118,13 +115,298 @@
   </si>
   <si>
     <t>left to right</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>ASTNode</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Subtype</t>
+  </si>
+  <si>
+    <t>||</t>
+  </si>
+  <si>
+    <t>|x|</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>!true</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>Unary</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>x + y</t>
+  </si>
+  <si>
+    <t>x - y</t>
+  </si>
+  <si>
+    <t>x * y</t>
+  </si>
+  <si>
+    <t>x / y</t>
+  </si>
+  <si>
+    <t>x % y</t>
+  </si>
+  <si>
+    <t>x ^ y</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Logical</t>
+  </si>
+  <si>
+    <t>Mathematical</t>
+  </si>
+  <si>
+    <t>&amp;&amp;</t>
+  </si>
+  <si>
+    <t>==</t>
+  </si>
+  <si>
+    <t>!=</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>Comparative</t>
+  </si>
+  <si>
+    <t>true &amp;&amp; false</t>
+  </si>
+  <si>
+    <t>true || false</t>
+  </si>
+  <si>
+    <t>x == y</t>
+  </si>
+  <si>
+    <t>x != y</t>
+  </si>
+  <si>
+    <t>x &lt; y</t>
+  </si>
+  <si>
+    <t>x &lt;= y</t>
+  </si>
+  <si>
+    <t>x &gt; y</t>
+  </si>
+  <si>
+    <t>x &gt;= y</t>
+  </si>
+  <si>
+    <t>~NOR</t>
+  </si>
+  <si>
+    <t>true ~NOR false</t>
+  </si>
+  <si>
+    <t>~NAND</t>
+  </si>
+  <si>
+    <t>true ~NAND false</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>x ? Y : z</t>
+  </si>
+  <si>
+    <t>Logical?</t>
+  </si>
+  <si>
+    <t>+=</t>
+  </si>
+  <si>
+    <t>-=</t>
+  </si>
+  <si>
+    <t>*=</t>
+  </si>
+  <si>
+    <t>/=</t>
+  </si>
+  <si>
+    <t>%=</t>
+  </si>
+  <si>
+    <t>^=</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>x += y</t>
+  </si>
+  <si>
+    <t>x -= y</t>
+  </si>
+  <si>
+    <t>x *= y</t>
+  </si>
+  <si>
+    <t>x /= y</t>
+  </si>
+  <si>
+    <t>x %= y</t>
+  </si>
+  <si>
+    <t>x ^= y</t>
+  </si>
+  <si>
+    <t>x = y</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>-&gt;</t>
+  </si>
+  <si>
+    <t>true -&gt; false</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>Accepts</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>boolean/number</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>boolean - any</t>
+  </si>
+  <si>
+    <t>x.y</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>Membership</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Ternary</t>
+  </si>
+  <si>
+    <t>Quaternary</t>
+  </si>
+  <si>
+    <t>Lexed</t>
+  </si>
+  <si>
+    <t>Parsed</t>
+  </si>
+  <si>
+    <t>try</t>
+  </si>
+  <si>
+    <t>catch</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>casting</t>
+  </si>
+  <si>
+    <t>int(x)</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>|x| () {} int() literal</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,13 +434,32 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -173,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -191,6 +492,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -510,7 +817,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +853,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,7 +867,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -574,7 +881,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -588,7 +895,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,7 +909,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,7 +923,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,7 +937,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -644,7 +951,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,7 +965,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,7 +979,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,13 +987,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,13 +1001,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -751,12 +1058,936 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="I21" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>